<commit_message>
AutoCommit_3 июля 2023 г. 14:41:12_SibNout2020
</commit_message>
<xml_diff>
--- a/2ИСИП-421/2ИСИП-421.xlsx
+++ b/2ИСИП-421/2ИСИП-421.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Git_Hub_V2\KipFin_Lab_2023_v0_Git0\2ИСИП-421\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE99BD1-A8AA-417A-942E-DD90187B421E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E19D7B-75CE-4A72-A614-107AAF4EA8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -590,10 +590,10 @@
   <dimension ref="A1:AA32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="X6" sqref="X6"/>
+      <selection pane="bottomRight" activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -686,19 +686,54 @@
       <c r="C4" s="4">
         <v>5</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0</v>
+      </c>
       <c r="T4" s="2"/>
       <c r="U4">
         <f>SUM(C4:S4)</f>
@@ -721,20 +756,57 @@
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0</v>
+      </c>
       <c r="T5" s="2"/>
       <c r="U5">
         <f t="shared" ref="U5:U31" si="0">SUM(C5:S5)</f>
@@ -799,8 +871,12 @@
       <c r="Q6" s="2">
         <v>5</v>
       </c>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
+      <c r="R6" s="2">
+        <v>0</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0</v>
+      </c>
       <c r="T6" s="2"/>
       <c r="U6">
         <f t="shared" si="0"/>
@@ -826,6 +902,9 @@
       <c r="D7">
         <v>5</v>
       </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
       <c r="F7">
         <v>5</v>
       </c>
@@ -865,7 +944,9 @@
       <c r="R7" s="2">
         <v>5</v>
       </c>
-      <c r="S7" s="2"/>
+      <c r="S7" s="2">
+        <v>0</v>
+      </c>
       <c r="T7" s="2"/>
       <c r="U7">
         <f t="shared" si="0"/>
@@ -888,19 +969,54 @@
       <c r="C8" s="4">
         <v>5</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
+        <v>0</v>
+      </c>
+      <c r="S8" s="2">
+        <v>0</v>
+      </c>
       <c r="T8" s="2"/>
       <c r="U8">
         <f t="shared" si="0"/>
@@ -953,7 +1069,9 @@
       <c r="M9" s="2">
         <v>5</v>
       </c>
-      <c r="N9" s="2"/>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
       <c r="O9" s="2">
         <v>5</v>
       </c>
@@ -991,6 +1109,15 @@
       <c r="C10" s="4">
         <v>5</v>
       </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
       <c r="G10" s="2">
         <v>5</v>
       </c>
@@ -1027,7 +1154,9 @@
       <c r="R10" s="2">
         <v>5</v>
       </c>
-      <c r="S10" s="2"/>
+      <c r="S10" s="2">
+        <v>0</v>
+      </c>
       <c r="T10" s="2"/>
       <c r="U10">
         <f t="shared" si="0"/>
@@ -1050,9 +1179,15 @@
       <c r="C11" s="4">
         <v>5</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0</v>
+      </c>
       <c r="G11" s="6">
         <v>5</v>
       </c>
@@ -1089,7 +1224,9 @@
       <c r="R11" s="6">
         <v>5</v>
       </c>
-      <c r="S11" s="2"/>
+      <c r="S11" s="2">
+        <v>0</v>
+      </c>
       <c r="T11" s="2"/>
       <c r="U11">
         <f t="shared" si="0"/>
@@ -1115,6 +1252,15 @@
       <c r="C12" s="4">
         <v>5</v>
       </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
       <c r="G12" s="2">
         <v>5</v>
       </c>
@@ -1218,8 +1364,12 @@
       <c r="Q13" s="2">
         <v>5</v>
       </c>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
+      <c r="R13" s="2">
+        <v>0</v>
+      </c>
+      <c r="S13" s="2">
+        <v>0</v>
+      </c>
       <c r="T13" s="2"/>
       <c r="U13">
         <f t="shared" si="0"/>
@@ -1242,19 +1392,54 @@
       <c r="C14" s="4">
         <v>5</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2">
+        <v>0</v>
+      </c>
+      <c r="S14" s="2">
+        <v>0</v>
+      </c>
       <c r="T14" s="2"/>
       <c r="U14">
         <f t="shared" si="0"/>
@@ -1322,8 +1507,12 @@
       <c r="Q15" s="2">
         <v>5</v>
       </c>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
+      <c r="R15" s="2">
+        <v>0</v>
+      </c>
+      <c r="S15" s="2">
+        <v>0</v>
+      </c>
       <c r="T15" s="2" t="s">
         <v>42</v>
       </c>
@@ -1391,8 +1580,12 @@
       <c r="Q16" s="2">
         <v>5</v>
       </c>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
+      <c r="R16" s="2">
+        <v>0</v>
+      </c>
+      <c r="S16" s="2">
+        <v>0</v>
+      </c>
       <c r="T16" s="2"/>
       <c r="U16">
         <f t="shared" si="0"/>
@@ -1457,8 +1650,12 @@
       <c r="Q17" s="2">
         <v>5</v>
       </c>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
+      <c r="R17" s="2">
+        <v>0</v>
+      </c>
+      <c r="S17" s="2">
+        <v>0</v>
+      </c>
       <c r="T17" s="2"/>
       <c r="U17">
         <f t="shared" si="0"/>
@@ -1481,6 +1678,15 @@
       <c r="C18" s="4">
         <v>5</v>
       </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
       <c r="G18" s="6">
         <v>5</v>
       </c>
@@ -1517,7 +1723,9 @@
       <c r="R18" s="6">
         <v>5</v>
       </c>
-      <c r="S18" s="2"/>
+      <c r="S18" s="2">
+        <v>0</v>
+      </c>
       <c r="T18" s="2"/>
       <c r="U18">
         <f t="shared" si="0"/>
@@ -1652,8 +1860,12 @@
       <c r="Q20" s="2">
         <v>5</v>
       </c>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
+      <c r="R20" s="2">
+        <v>0</v>
+      </c>
+      <c r="S20" s="2">
+        <v>0</v>
+      </c>
       <c r="T20" s="2"/>
       <c r="U20">
         <f t="shared" si="0"/>
@@ -1858,8 +2070,12 @@
       <c r="Q23" s="2">
         <v>5</v>
       </c>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
+      <c r="R23" s="2">
+        <v>0</v>
+      </c>
+      <c r="S23" s="2">
+        <v>0</v>
+      </c>
       <c r="T23" s="2"/>
       <c r="U23">
         <f t="shared" si="0"/>
@@ -1958,6 +2174,9 @@
       <c r="E25">
         <v>5</v>
       </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
       <c r="G25" s="2">
         <v>5</v>
       </c>
@@ -1985,7 +2204,9 @@
       <c r="O25" s="2">
         <v>5</v>
       </c>
-      <c r="P25" s="2"/>
+      <c r="P25" s="2">
+        <v>0</v>
+      </c>
       <c r="Q25" s="2">
         <v>5</v>
       </c>
@@ -2132,7 +2353,9 @@
       <c r="R27" s="2">
         <v>5</v>
       </c>
-      <c r="S27" s="2"/>
+      <c r="S27" s="2">
+        <v>0</v>
+      </c>
       <c r="T27" s="2"/>
       <c r="U27">
         <f t="shared" si="0"/>
@@ -2234,7 +2457,9 @@
       <c r="F29">
         <v>5</v>
       </c>
-      <c r="G29" s="2"/>
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
       <c r="H29" s="2">
         <v>5</v>
       </c>
@@ -2265,7 +2490,9 @@
       <c r="Q29" s="2">
         <v>5</v>
       </c>
-      <c r="R29" s="2"/>
+      <c r="R29" s="2">
+        <v>0</v>
+      </c>
       <c r="S29" s="2">
         <v>5</v>
       </c>
@@ -2288,19 +2515,36 @@
       <c r="B30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="2"/>
+      <c r="C30" s="2">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
       <c r="G30" s="2">
         <v>5</v>
       </c>
-      <c r="H30" s="2"/>
+      <c r="H30" s="2">
+        <v>0</v>
+      </c>
       <c r="I30" s="2">
         <v>5</v>
       </c>
       <c r="J30" s="2">
         <v>5</v>
       </c>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
+      <c r="K30" s="2">
+        <v>0</v>
+      </c>
+      <c r="L30" s="2">
+        <v>0</v>
+      </c>
       <c r="M30" s="2">
         <v>5</v>
       </c>
@@ -2334,7 +2578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:27" ht="51" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" ht="22" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -2344,6 +2588,15 @@
       <c r="C31" s="4">
         <v>5</v>
       </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>5</v>
+      </c>
       <c r="G31" s="2">
         <v>5</v>
       </c>
@@ -2377,14 +2630,18 @@
       <c r="Q31" s="2">
         <v>5</v>
       </c>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
+      <c r="R31" s="2">
+        <v>0</v>
+      </c>
+      <c r="S31" s="2">
+        <v>0</v>
+      </c>
       <c r="T31" s="2" t="s">
         <v>42</v>
       </c>
       <c r="U31">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="V31" s="2" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
AutoCommit_3 июля 2023 г. 14:46:55_SibNout2020
</commit_message>
<xml_diff>
--- a/2ИСИП-421/2ИСИП-421.xlsx
+++ b/2ИСИП-421/2ИСИП-421.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Git_Hub_V2\KipFin_Lab_2023_v0_Git0\2ИСИП-421\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E19D7B-75CE-4A72-A614-107AAF4EA8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DDBA73-3366-4B04-9093-05AB5E2F2514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -263,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -283,6 +283,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -590,10 +593,10 @@
   <dimension ref="A1:AA32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S1" sqref="S1"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="C4:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -683,10 +686,10 @@
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4">
-        <v>5</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="9">
+        <v>5</v>
+      </c>
+      <c r="D4" s="7">
         <v>0</v>
       </c>
       <c r="E4">
@@ -756,57 +759,21 @@
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2">
-        <v>0</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0</v>
-      </c>
-      <c r="O5" s="2">
-        <v>0</v>
-      </c>
-      <c r="P5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0</v>
-      </c>
-      <c r="R5" s="2">
-        <v>0</v>
-      </c>
-      <c r="S5" s="2">
-        <v>0</v>
-      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="7"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
       <c r="T5" s="2"/>
       <c r="U5">
         <f t="shared" ref="U5:U31" si="0">SUM(C5:S5)</f>
@@ -826,10 +793,10 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="4">
-        <v>5</v>
-      </c>
-      <c r="D6">
+      <c r="C6" s="9">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7">
         <v>5</v>
       </c>
       <c r="E6">
@@ -896,10 +863,10 @@
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="4">
-        <v>5</v>
-      </c>
-      <c r="D7">
+      <c r="C7" s="9">
+        <v>5</v>
+      </c>
+      <c r="D7" s="7">
         <v>5</v>
       </c>
       <c r="E7">
@@ -966,10 +933,10 @@
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="4">
-        <v>5</v>
-      </c>
-      <c r="D8">
+      <c r="C8" s="9">
+        <v>5</v>
+      </c>
+      <c r="D8" s="7">
         <v>0</v>
       </c>
       <c r="E8">
@@ -1036,10 +1003,10 @@
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="4">
-        <v>5</v>
-      </c>
-      <c r="D9">
+      <c r="C9" s="9">
+        <v>5</v>
+      </c>
+      <c r="D9" s="7">
         <v>5</v>
       </c>
       <c r="E9">
@@ -1106,10 +1073,10 @@
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="4">
-        <v>5</v>
-      </c>
-      <c r="D10">
+      <c r="C10" s="9">
+        <v>5</v>
+      </c>
+      <c r="D10" s="7">
         <v>0</v>
       </c>
       <c r="E10">
@@ -1176,7 +1143,7 @@
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="9">
         <v>5</v>
       </c>
       <c r="D11" s="7">
@@ -1249,10 +1216,10 @@
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="4">
-        <v>5</v>
-      </c>
-      <c r="D12">
+      <c r="C12" s="9">
+        <v>5</v>
+      </c>
+      <c r="D12" s="7">
         <v>0</v>
       </c>
       <c r="E12">
@@ -1319,10 +1286,10 @@
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="4">
-        <v>5</v>
-      </c>
-      <c r="D13">
+      <c r="C13" s="9">
+        <v>5</v>
+      </c>
+      <c r="D13" s="7">
         <v>5</v>
       </c>
       <c r="E13">
@@ -1389,10 +1356,10 @@
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="4">
-        <v>5</v>
-      </c>
-      <c r="D14">
+      <c r="C14" s="9">
+        <v>5</v>
+      </c>
+      <c r="D14" s="7">
         <v>0</v>
       </c>
       <c r="E14">
@@ -1462,10 +1429,10 @@
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="2">
-        <v>5</v>
-      </c>
-      <c r="D15">
+      <c r="C15" s="9">
+        <v>5</v>
+      </c>
+      <c r="D15" s="7">
         <v>5</v>
       </c>
       <c r="E15">
@@ -1535,10 +1502,10 @@
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="4">
-        <v>5</v>
-      </c>
-      <c r="D16">
+      <c r="C16" s="9">
+        <v>5</v>
+      </c>
+      <c r="D16" s="7">
         <v>5</v>
       </c>
       <c r="E16">
@@ -1605,10 +1572,10 @@
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="4">
-        <v>5</v>
-      </c>
-      <c r="D17">
+      <c r="C17" s="9">
+        <v>5</v>
+      </c>
+      <c r="D17" s="7">
         <v>5</v>
       </c>
       <c r="E17">
@@ -1675,10 +1642,10 @@
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="4">
-        <v>5</v>
-      </c>
-      <c r="D18">
+      <c r="C18" s="9">
+        <v>5</v>
+      </c>
+      <c r="D18" s="7">
         <v>0</v>
       </c>
       <c r="E18">
@@ -1745,10 +1712,10 @@
       <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="4">
-        <v>5</v>
-      </c>
-      <c r="D19">
+      <c r="C19" s="9">
+        <v>5</v>
+      </c>
+      <c r="D19" s="7">
         <v>5</v>
       </c>
       <c r="E19">
@@ -1815,10 +1782,10 @@
       <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="4">
-        <v>5</v>
-      </c>
-      <c r="D20">
+      <c r="C20" s="9">
+        <v>5</v>
+      </c>
+      <c r="D20" s="7">
         <v>5</v>
       </c>
       <c r="E20">
@@ -1885,10 +1852,10 @@
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="4">
-        <v>5</v>
-      </c>
-      <c r="D21">
+      <c r="C21" s="9">
+        <v>5</v>
+      </c>
+      <c r="D21" s="7">
         <v>5</v>
       </c>
       <c r="E21">
@@ -1955,10 +1922,10 @@
       <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="4">
-        <v>5</v>
-      </c>
-      <c r="D22">
+      <c r="C22" s="9">
+        <v>5</v>
+      </c>
+      <c r="D22" s="7">
         <v>5</v>
       </c>
       <c r="E22">
@@ -2025,10 +1992,10 @@
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="4">
-        <v>5</v>
-      </c>
-      <c r="D23">
+      <c r="C23" s="9">
+        <v>5</v>
+      </c>
+      <c r="D23" s="7">
         <v>5</v>
       </c>
       <c r="E23">
@@ -2095,10 +2062,10 @@
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="4">
-        <v>5</v>
-      </c>
-      <c r="D24">
+      <c r="C24" s="9">
+        <v>5</v>
+      </c>
+      <c r="D24" s="7">
         <v>5</v>
       </c>
       <c r="E24">
@@ -2165,10 +2132,10 @@
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="4">
-        <v>5</v>
-      </c>
-      <c r="D25">
+      <c r="C25" s="9">
+        <v>5</v>
+      </c>
+      <c r="D25" s="7">
         <v>5</v>
       </c>
       <c r="E25">
@@ -2235,10 +2202,10 @@
       <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="4">
-        <v>5</v>
-      </c>
-      <c r="D26">
+      <c r="C26" s="9">
+        <v>5</v>
+      </c>
+      <c r="D26" s="7">
         <v>5</v>
       </c>
       <c r="E26">
@@ -2305,10 +2272,10 @@
       <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="4">
-        <v>5</v>
-      </c>
-      <c r="D27">
+      <c r="C27" s="9">
+        <v>5</v>
+      </c>
+      <c r="D27" s="7">
         <v>5</v>
       </c>
       <c r="E27">
@@ -2375,10 +2342,10 @@
       <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="4">
-        <v>5</v>
-      </c>
-      <c r="D28">
+      <c r="C28" s="9">
+        <v>5</v>
+      </c>
+      <c r="D28" s="7">
         <v>5</v>
       </c>
       <c r="E28">
@@ -2445,10 +2412,10 @@
       <c r="B29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="4">
-        <v>5</v>
-      </c>
-      <c r="D29">
+      <c r="C29" s="9">
+        <v>5</v>
+      </c>
+      <c r="D29" s="7">
         <v>5</v>
       </c>
       <c r="E29">
@@ -2515,10 +2482,10 @@
       <c r="B30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="2">
-        <v>0</v>
-      </c>
-      <c r="D30">
+      <c r="C30" s="9">
+        <v>0</v>
+      </c>
+      <c r="D30" s="7">
         <v>0</v>
       </c>
       <c r="E30">
@@ -2585,10 +2552,10 @@
       <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="4">
-        <v>5</v>
-      </c>
-      <c r="D31">
+      <c r="C31" s="9">
+        <v>5</v>
+      </c>
+      <c r="D31" s="7">
         <v>5</v>
       </c>
       <c r="E31">

</xml_diff>